<commit_message>
Incorporated data provider's changes to Mac Low CLR and OLR, finalized for test ingest
</commit_message>
<xml_diff>
--- a/mac-low/CLR/CLR_standard_input_mac_low.xlsx
+++ b/mac-low/CLR/CLR_standard_input_mac_low.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\mac-low-metadata\CLR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\MacLowAudio\CLR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="11835" tabRatio="402"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="11835" tabRatio="372"/>
   </bookViews>
   <sheets>
     <sheet name="Item description" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="644">
   <si>
     <t>text</t>
   </si>
@@ -2059,12 +2059,6 @@
     <t>001</t>
   </si>
   <si>
-    <t>Mac Low Audio Recordings</t>
-  </si>
-  <si>
-    <t>circa 1955 to 1993</t>
-  </si>
-  <si>
     <t>1955-01-01</t>
   </si>
   <si>
@@ -2075,13 +2069,39 @@
   </si>
   <si>
     <t>American poetry</t>
+  </si>
+  <si>
+    <t>From the &lt;a href="http://library.ucsd.edu/speccoll/findingaids/mss0180.html"&gt;Jackson Mac Low Papers&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>Jackson Mac Low Papers @ http://library.ucsd.edu/speccoll/findingaids/mss0180.html</t>
+  </si>
+  <si>
+    <t>Jackson Mac Low Sound Recordings</t>
+  </si>
+  <si>
+    <t>A collection of sound recordings of poetry performances by Jackson Mac Low, digitized from tape reels found in his papers. The recordings feature words and music performed by Mac Low and various collaborators.</t>
+  </si>
+  <si>
+    <t>circa 1955-1993</t>
+  </si>
+  <si>
+    <t>CLR_mss0180_b236_f15.tif</t>
+  </si>
+  <si>
+    <t>A collection of sound recordings of poetry performances by Jackson Mac Low, digitized from original tape reels found in his papers. Due to copyright restrictions, access to recordings is limited to the Special Collections &amp; Archives reading room. Researchers may contact SC&amp;A with futher questions regarding access.
+The recordings include performances of the titles A Vocabulary for Sharon Belle Mattlin, Age of Anxiety, Asymmetries 1-190, Milarepa Gatha, The 5th Biblical Poem, and The Text on the Opposite Page, among many others. Multiple recordings may feature recitation of the same poem, but each performance is unique. The sound files feature words and music performed by Mac Low and various colleagues, friends, and family, including Paul Blackburn, Spencer Holst, Jerome Rothenberg, Armand Schwerner, Anne Tardos and Diane Wakoski.
+The majority of the original reel-to-reel recordings are labeled with unique "RJ" and "RM" numbers that follow Mac Low's own indexing system. These numbers have been preserved in the titles of the recordings, and reflect the original order of the sound library, which was mostly chronological.</t>
+  </si>
+  <si>
+    <t>Mac Low, Jackson | Blackburn, Paul | Holst, Spencer | Rothenberg, Jerome, 1931- | Schwerner, Armand | Tardos, Anne | Wakoski, Diane</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2307,6 +2327,13 @@
     <font>
       <sz val="11"/>
       <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2706,7 +2733,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2752,6 +2779,9 @@
     <xf numFmtId="49" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3117,10 +3147,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3130,13 +3160,13 @@
     <col min="3" max="3" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" style="3" customWidth="1"/>
     <col min="5" max="5" width="51.5703125" style="3" customWidth="1"/>
-    <col min="6" max="7" width="45.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="45.5703125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="53.140625" style="3" customWidth="1"/>
-    <col min="12" max="13" width="39.140625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="42.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="45.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="45.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="53.140625" style="3" customWidth="1"/>
+    <col min="11" max="12" width="39.140625" style="3" customWidth="1"/>
+    <col min="13" max="14" width="42.85546875" style="3" customWidth="1"/>
     <col min="15" max="15" width="84.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3160,37 +3190,40 @@
         <v>95</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>525</v>
+        <v>486</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>486</v>
+        <v>5</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="J1" s="17" t="s">
         <v>620</v>
       </c>
+      <c r="K1" s="16" t="s">
+        <v>3</v>
+      </c>
       <c r="L1" s="16" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>490</v>
+        <v>459</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="O1" s="16" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="382.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>631</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>641</v>
+      </c>
       <c r="C2" s="3" t="s">
         <v>370</v>
       </c>
@@ -3198,23 +3231,42 @@
         <v>357</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>632</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="I2" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>639</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>642</v>
+      </c>
+      <c r="L2" s="23" t="s">
         <v>636</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>633</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>634</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>635</v>
       </c>
       <c r="N2" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>637</v>
       </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -3225,7 +3277,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'CV values'!$C$2:$C$15</xm:f>
@@ -3246,21 +3298,15 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
-            <xm:f>'Select-a-header values'!$C$1:$C$185</xm:f>
+            <xm:f>'Select-a-header values'!$D$1:$D$6</xm:f>
           </x14:formula1>
           <xm:sqref>G1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
-            <xm:f>'Select-a-header values'!$D$1:$D$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>H1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>N1</xm:sqref>
+          <xm:sqref>M1:N1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
@@ -3278,13 +3324,7 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$E$1:$E$34</xm:f>
           </x14:formula1>
-          <xm:sqref>L1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'Select-a-header values'!$F$1:$F$21</xm:f>
-          </x14:formula1>
-          <xm:sqref>M1</xm:sqref>
+          <xm:sqref>K1:L1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Finalized CLR for production ingest
</commit_message>
<xml_diff>
--- a/mac-low/CLR/CLR_standard_input_mac_low.xlsx
+++ b/mac-low/CLR/CLR_standard_input_mac_low.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\MacLowAudio\CLR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\MacLowAudio\CLR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2071,9 +2071,6 @@
     <t>American poetry</t>
   </si>
   <si>
-    <t>From the &lt;a href="http://library.ucsd.edu/speccoll/findingaids/mss0180.html"&gt;Jackson Mac Low Papers&lt;/a&gt;.</t>
-  </si>
-  <si>
     <t>Jackson Mac Low Papers @ http://library.ucsd.edu/speccoll/findingaids/mss0180.html</t>
   </si>
   <si>
@@ -2089,12 +2086,15 @@
     <t>CLR_mss0180_b236_f15.tif</t>
   </si>
   <si>
-    <t>A collection of sound recordings of poetry performances by Jackson Mac Low, digitized from original tape reels found in his papers. Due to copyright restrictions, access to recordings is limited to the Special Collections &amp; Archives reading room. Researchers may contact SC&amp;A with futher questions regarding access.
+    <t>Mac Low, Jackson | Blackburn, Paul | Holst, Spencer | Rothenberg, Jerome, 1931- | Schwerner, Armand | Tardos, Anne | Wakoski, Diane</t>
+  </si>
+  <si>
+    <t>A collection of sound recordings of poetry performances by Jackson Mac Low, digitized from original tape reels found in his papers. Due to copyright restrictions, access to recordings is limited to the Special Collections &amp; Archives reading room. Researchers may contact Special Collections &amp; Archives to inquire about access to particular performances.
 The recordings include performances of the titles A Vocabulary for Sharon Belle Mattlin, Age of Anxiety, Asymmetries 1-190, Milarepa Gatha, The 5th Biblical Poem, and The Text on the Opposite Page, among many others. Multiple recordings may feature recitation of the same poem, but each performance is unique. The sound files feature words and music performed by Mac Low and various colleagues, friends, and family, including Paul Blackburn, Spencer Holst, Jerome Rothenberg, Armand Schwerner, Anne Tardos and Diane Wakoski.
 The majority of the original reel-to-reel recordings are labeled with unique "RJ" and "RM" numbers that follow Mac Low's own indexing system. These numbers have been preserved in the titles of the recordings, and reflect the original order of the sound library, which was mostly chronological.</t>
   </si>
   <si>
-    <t>Mac Low, Jackson | Blackburn, Paul | Holst, Spencer | Rothenberg, Jerome, 1931- | Schwerner, Armand | Tardos, Anne | Wakoski, Diane</t>
+    <t>From the &lt;a href="http://library.ucsd.edu/speccoll/findingaids/mss0180.html"&gt;Jackson Mac Low Papers&lt;/a&gt;. MSS 180. Special Collections &amp; Archives, UC San Diego.</t>
   </si>
 </sst>
 </file>
@@ -3149,8 +3149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3217,12 +3217,12 @@
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="382.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="395.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>631</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>370</v>
@@ -3231,13 +3231,13 @@
         <v>357</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>634</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>632</v>
@@ -3246,22 +3246,22 @@
         <v>633</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>642</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>636</v>
+        <v>643</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>635</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>